<commit_message>
Hangman-React primer approach, más varios
</commit_message>
<xml_diff>
--- a/staff/ariel/Project/contenido.xlsx
+++ b/staff/ariel/Project/contenido.xlsx
@@ -1,23 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10523"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arielcima/Skylab/skylab-partTimeFront-201805/staff/ariel/Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4CA8EB6-6F29-9B47-B4AE-31B9CB2DF14C}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A782228-7271-234A-AB15-37E014FE3E6A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="280" yWindow="460" windowWidth="26740" windowHeight="14420" xr2:uid="{C3C59CB8-E142-534B-B54B-2F07D83096D0}"/>
+    <workbookView xWindow="280" yWindow="460" windowWidth="26740" windowHeight="14420" activeTab="1" xr2:uid="{C3C59CB8-E142-534B-B54B-2F07D83096D0}"/>
   </bookViews>
   <sheets>
-    <sheet name="Gral" sheetId="3" r:id="rId1"/>
-    <sheet name="Landing" sheetId="1" r:id="rId2"/>
-    <sheet name="Main" sheetId="2" r:id="rId3"/>
+    <sheet name="PROCESS" sheetId="4" r:id="rId1"/>
+    <sheet name="MAIN" sheetId="9" r:id="rId2"/>
+    <sheet name="GRAL" sheetId="3" r:id="rId3"/>
+    <sheet name="BOARD" sheetId="1" r:id="rId4"/>
+    <sheet name="J'ers" sheetId="2" r:id="rId5"/>
+    <sheet name="PRIV AREA" sheetId="7" r:id="rId6"/>
+    <sheet name="CREATE" sheetId="5" r:id="rId7"/>
+    <sheet name="SIGNIN" sheetId="6" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,22 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
-  <si>
-    <t>join</t>
-  </si>
-  <si>
-    <t>enter email</t>
-  </si>
-  <si>
-    <t>enter password</t>
-  </si>
-  <si>
-    <t>create</t>
-  </si>
-  <si>
-    <t>verify email</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="73">
   <si>
     <t>Registro usuario</t>
   </si>
@@ -93,13 +83,184 @@
   </si>
   <si>
     <t>Downloads</t>
+  </si>
+  <si>
+    <t>REGISTRATION FORM FOR AMPLE JAM REQUEST</t>
+  </si>
+  <si>
+    <t>Dinamic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Contract autofill</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Monthly rent chart</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Deposit status</t>
+  </si>
+  <si>
+    <t>Static</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    House rules</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Getting here</t>
+  </si>
+  <si>
+    <t>"PRIV AREA" CONFIG</t>
+  </si>
+  <si>
+    <t>ACCEPTANCE REPLY
+(w link to Ample's Board)</t>
+  </si>
+  <si>
+    <t>Booking confirmation
+(name and email)</t>
+  </si>
+  <si>
+    <t>Manual validation</t>
+  </si>
+  <si>
+    <t>Ample's invitation 
+SIGN IN LINK + REG FORM</t>
+  </si>
+  <si>
+    <t>MUST</t>
+  </si>
+  <si>
+    <t>SHOULD</t>
+  </si>
+  <si>
+    <t>COULD</t>
+  </si>
+  <si>
+    <t>WOULD</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Jammers post</t>
+  </si>
+  <si>
+    <t>Admin post</t>
+  </si>
+  <si>
+    <t>Autoposts</t>
+  </si>
+  <si>
+    <t>Programmable posts</t>
+  </si>
+  <si>
+    <t>Default Show profile</t>
+  </si>
+  <si>
+    <t>Select not to show profile</t>
+  </si>
+  <si>
+    <t>Create Jam with memebers</t>
+  </si>
+  <si>
+    <t>Private chat</t>
+  </si>
+  <si>
+    <t>JAMMERS / MEMBERS</t>
+  </si>
+  <si>
+    <t>CREATE</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Name *</t>
+  </si>
+  <si>
+    <t>Description (*)</t>
+  </si>
+  <si>
+    <t>Location (*)</t>
+  </si>
+  <si>
+    <t>End Date and time (*)</t>
+  </si>
+  <si>
+    <t>Start Date and time (*)</t>
+  </si>
+  <si>
+    <t>Invite (email with link)</t>
+  </si>
+  <si>
+    <t>Wifi restriction</t>
+  </si>
+  <si>
+    <t>Location restriction</t>
+  </si>
+  <si>
+    <t>Reg Form creation</t>
+  </si>
+  <si>
+    <t>Jam picture (*)</t>
+  </si>
+  <si>
+    <t>SIGN IN</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Verification process</t>
+  </si>
+  <si>
+    <t>Captcha security</t>
+  </si>
+  <si>
+    <t>Profile edit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Email</t>
+  </si>
+  <si>
+    <t>Private settings</t>
+  </si>
+  <si>
+    <t>JAM'S PRIV AREA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Possibility of no display profile in group</t>
+  </si>
+  <si>
+    <t>Priv Jam info</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Contract (pdf access)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Month rental scheme and evolution</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Contract download</t>
+  </si>
+  <si>
+    <t>BOARD</t>
+  </si>
+  <si>
+    <t>MAIN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This is a list of persons and groups </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -107,13 +268,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="4">
@@ -169,17 +344,36 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -494,11 +688,159 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BE99202-42C8-D246-AAF4-55EBB262EC95}">
+  <dimension ref="B3:O14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" style="5"/>
+    <col min="2" max="2" width="20" style="5" customWidth="1"/>
+    <col min="3" max="4" width="5.33203125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="20" style="5" customWidth="1"/>
+    <col min="6" max="6" width="5.33203125" style="5" customWidth="1"/>
+    <col min="7" max="7" width="20" style="5" customWidth="1"/>
+    <col min="8" max="8" width="5.33203125" style="5" customWidth="1"/>
+    <col min="9" max="9" width="20" style="5" customWidth="1"/>
+    <col min="10" max="10" width="5.33203125" style="5" customWidth="1"/>
+    <col min="11" max="11" width="20" style="5" customWidth="1"/>
+    <col min="12" max="12" width="5.33203125" style="5" customWidth="1"/>
+    <col min="13" max="13" width="20" style="5" customWidth="1"/>
+    <col min="14" max="14" width="5.33203125" style="5" customWidth="1"/>
+    <col min="15" max="15" width="20" style="5" customWidth="1"/>
+    <col min="16" max="16384" width="10.83203125" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:15" ht="64" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="M3" s="6"/>
+      <c r="O3" s="6"/>
+    </row>
+    <row r="5" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="I5" s="8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="I6" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="I7" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="I8" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="I10" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="I11" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="I12" s="8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="I13" s="8"/>
+    </row>
+    <row r="14" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="I14" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BF18D40-6E20-AE47-9220-46669BAF7859}">
+  <dimension ref="C2:G8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="7" width="11.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C4" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D5" s="9"/>
+    </row>
+    <row r="6" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="F6" s="9"/>
+    </row>
+    <row r="7" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="G7" s="9"/>
+    </row>
+    <row r="8" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="G8" s="9"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A1CA7D2-85C9-0544-8551-3CE116867EE0}">
   <dimension ref="B4:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="207" zoomScaleNormal="207" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView topLeftCell="A3" zoomScale="207" zoomScaleNormal="207" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -509,85 +851,85 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B5" s="2"/>
+      <c r="C5" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B6" s="2"/>
+      <c r="C6" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C7" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B8" s="2"/>
+      <c r="C8" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B9" s="2"/>
+      <c r="C9" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B10" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B11" s="2"/>
+      <c r="C11" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B12" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B5" s="1"/>
-      <c r="C5" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B6" s="1"/>
-      <c r="C6" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B7" s="1" t="s">
+      <c r="C12" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B13" s="2"/>
+      <c r="C13" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B8" s="1"/>
-      <c r="C8" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B9" s="1"/>
-      <c r="C9" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B10" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B11" s="1"/>
-      <c r="C11" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B12" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B13" s="1"/>
-      <c r="C13" s="2" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B14" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>20</v>
+        <v>14</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B15" s="4"/>
-      <c r="C15" s="2" t="s">
-        <v>21</v>
+      <c r="C15" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -602,49 +944,66 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3594728-C2B3-7E46-BDE6-81EFAB90C096}">
-  <dimension ref="B3:C10"/>
+  <dimension ref="C4:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="18.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="C4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C4" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C5" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B7" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C6" t="s">
+        <v>35</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C7" t="s">
+        <v>37</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C8" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="C9" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="C10" t="s">
-        <v>4</v>
+        <v>38</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -652,16 +1011,465 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C5D6A1D-B023-2147-AD40-EE80969E5930}">
-  <dimension ref="A1"/>
+  <dimension ref="C3:M7"/>
   <sheetViews>
-    <sheetView topLeftCell="A77" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="3" max="3" width="24.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="13" width="10.83203125" style="9"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C3" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C5" t="s">
+        <v>40</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C7" t="s">
+        <v>42</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B700D30D-4EE5-3643-815E-8F443882E2B2}">
+  <dimension ref="C3:M13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="35.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="13" width="10.83203125" style="9"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C3" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C5" t="s">
+        <v>61</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C6" t="s">
+        <v>62</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C8" t="s">
+        <v>65</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C9" t="s">
+        <v>66</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C10" t="s">
+        <v>67</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C11" t="s">
+        <v>69</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C12" t="s">
+        <v>68</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C13" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{841FB19C-6CE2-9545-81C4-F0C3FF67A91B}">
+  <dimension ref="C3:M86"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="24.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="13" width="10.83203125" style="9"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C3" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C6" t="s">
+        <v>55</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C7" t="s">
+        <v>50</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C8" t="s">
+        <v>49</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C9" t="s">
+        <v>48</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C10" t="s">
+        <v>54</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C11" t="s">
+        <v>51</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C12" t="s">
+        <v>52</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C13" t="s">
+        <v>53</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="82" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C82" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="D82" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E82" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="F82" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="G82" s="11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="83" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C83" t="s">
+        <v>39</v>
+      </c>
+      <c r="D83" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="84" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C84" t="s">
+        <v>40</v>
+      </c>
+      <c r="G84" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="85" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C85" t="s">
+        <v>41</v>
+      </c>
+      <c r="E85" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="86" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C86" t="s">
+        <v>42</v>
+      </c>
+      <c r="E86" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BE57317-038A-764A-9820-2888368BDB04}">
+  <dimension ref="C3:M86"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="24.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="13" width="10.83203125" style="9"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C3" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C6" t="s">
+        <v>59</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C7" t="s">
+        <v>58</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="82" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C82" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="D82" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E82" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="F82" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="G82" s="11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="83" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C83" t="s">
+        <v>39</v>
+      </c>
+      <c r="D83" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="84" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C84" t="s">
+        <v>40</v>
+      </c>
+      <c r="G84" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="85" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C85" t="s">
+        <v>41</v>
+      </c>
+      <c r="E85" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="86" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C86" t="s">
+        <v>42</v>
+      </c>
+      <c r="E86" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>